<commit_message>
valid login page for testcase1
</commit_message>
<xml_diff>
--- a/data/input.xlsx
+++ b/data/input.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\B78\Workspace\b78framework\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7349A2A-C916-431E-A1E3-66F126D299A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{591A5C73-01A8-4B4F-A518-E196F8307C34}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Test1" sheetId="1" r:id="rId1"/>
+    <sheet name="ValidLogin" sheetId="2" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -27,16 +27,16 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
-    <t>username</t>
+    <t>UserName</t>
   </si>
   <si>
-    <t>password</t>
+    <t>Password</t>
   </si>
   <si>
-    <t>bhanu</t>
+    <t>admin</t>
   </si>
   <si>
-    <t>akshara</t>
+    <t>manager</t>
   </si>
 </sst>
 </file>
@@ -353,11 +353,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{072D2723-967F-4629-AC7A-2D368F1CECEE}">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="235" zoomScaleNormal="235" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>